<commit_message>
Add field email into structure of  student file
</commit_message>
<xml_diff>
--- a/csv_files/ImportStudent.xlsx
+++ b/csv_files/ImportStudent.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NguyenKJ\Desktop\HK1 2023 2024\Web nâng cao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\university\Final\csv_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5342024-FBC5-4875-95E8-B455436D5F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D471D3C-58A8-471B-B95A-903DDB5AD5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3432" yWindow="1200" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>studentId</t>
   </si>
@@ -46,16 +46,33 @@
   </si>
   <si>
     <t>Lê Công</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>nguyen@gmail.com</t>
+  </si>
+  <si>
+    <t>dat@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,13 +95,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -363,48 +383,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C3"/>
+      <selection activeCell="X14" sqref="X14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>20120537</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>20120456</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{1C83A2BF-FF1F-48A8-953D-42C8D2C81C1A}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{C7CAA933-2DBD-4B60-A283-EA630E038A8C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>